<commit_message>
README benchmark table update.
</commit_message>
<xml_diff>
--- a/pose_estimators.xlsx
+++ b/pose_estimators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\codes\Pose-Estimation-Benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28865039-DA07-4CAE-B7C9-A82E6785F724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49179E4C-CA1B-4289-9CFE-060CF53BBC26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{458BF1DC-8382-4D06-8CC6-A82EA8C2DB25}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Paper</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>***</t>
+  </si>
+  <si>
+    <t>5.28</t>
   </si>
 </sst>
 </file>
@@ -541,7 +544,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +637,9 @@
       <c r="C6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>